<commit_message>
kakaofriends - erd 설계 ver2.01
</commit_message>
<xml_diff>
--- a/Excel 정리/신규상품 관련.xlsx
+++ b/Excel 정리/신규상품 관련.xlsx
@@ -54,10 +54,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>배송사 고유번호</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>LED 시계_라이언&amp;춘식이</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -178,6 +174,10 @@
   </si>
   <si>
     <t>COOL한 파자마 모음</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>분류코드</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -202,7 +202,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -212,6 +212,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -245,7 +251,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -253,6 +259,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -556,22 +568,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M14"/>
+  <dimension ref="A1:P14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="14.875" customWidth="1"/>
-    <col min="3" max="3" width="44.75" customWidth="1"/>
-    <col min="4" max="11" width="14.875" customWidth="1"/>
-    <col min="12" max="12" width="36" customWidth="1"/>
+    <col min="3" max="3" width="22" customWidth="1"/>
+    <col min="4" max="4" width="68.25" customWidth="1"/>
+    <col min="5" max="11" width="14.875" customWidth="1"/>
+    <col min="12" max="12" width="12.375" customWidth="1"/>
     <col min="13" max="13" width="53.75" customWidth="1"/>
+    <col min="14" max="14" width="36.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -579,417 +593,474 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+    </row>
+    <row r="2" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="M1" s="1" t="s">
+      <c r="E2" s="3">
+        <v>450</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3">
+        <v>35000</v>
+      </c>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
+      <c r="N2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+    </row>
+    <row r="3" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>9</v>
+      </c>
+      <c r="B3" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="1">
+      <c r="C3" s="3">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="3">
+        <v>450</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="1">
-        <v>450</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="G3" s="3"/>
+      <c r="H3" s="3">
+        <v>35000</v>
+      </c>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+    </row>
+    <row r="4" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>9</v>
+      </c>
+      <c r="B4" s="3">
+        <v>2</v>
+      </c>
+      <c r="C4" s="3">
+        <v>2</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1">
-        <v>35000</v>
-      </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1">
+      <c r="E4" s="3">
+        <v>550</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3">
+        <v>49000</v>
+      </c>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+    </row>
+    <row r="5" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
         <v>1</v>
       </c>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="M2" s="1" t="s">
+      <c r="B5" s="3">
+        <v>2</v>
+      </c>
+      <c r="C5" s="3">
+        <v>2</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="3">
+        <v>550</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3">
+        <v>49000</v>
+      </c>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
+      <c r="N5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+    </row>
+    <row r="6" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
         <v>9</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B6" s="3">
+        <v>3</v>
+      </c>
+      <c r="C6" s="3">
+        <v>3</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="3">
+        <v>2000</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3">
+        <v>24000</v>
+      </c>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+    </row>
+    <row r="7" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
         <v>1</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="B7" s="3">
+        <v>3</v>
+      </c>
+      <c r="C7" s="3">
+        <v>4</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="3">
+        <v>1200</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3">
+        <v>39000</v>
+      </c>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+    </row>
+    <row r="8" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <v>9</v>
+      </c>
+      <c r="B8" s="3">
+        <v>4</v>
+      </c>
+      <c r="C8" s="3">
+        <v>4</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="3">
+        <v>1200</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3">
+        <v>39000</v>
+      </c>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+    </row>
+    <row r="9" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
+        <v>1</v>
+      </c>
+      <c r="B9" s="3">
+        <v>4</v>
+      </c>
+      <c r="C9" s="3">
+        <v>5</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="3">
+        <v>550</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3">
+        <v>39000</v>
+      </c>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="N9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+    </row>
+    <row r="10" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3">
+        <v>5</v>
+      </c>
+      <c r="C10" s="3">
+        <v>5</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="3">
+        <v>550</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3">
+        <v>39000</v>
+      </c>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+    </row>
+    <row r="11" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
         <v>10</v>
       </c>
-      <c r="D3" s="1">
-        <v>450</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1">
-        <v>35000</v>
-      </c>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1">
+      <c r="B11" s="3">
         <v>1</v>
       </c>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
-        <v>9</v>
-      </c>
-      <c r="B4" s="1">
-        <v>2</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="C11" s="3">
+        <v>6</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="3">
+        <v>5800</v>
+      </c>
+      <c r="F11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="1">
-        <v>550</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1">
-        <v>49000</v>
-      </c>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
-        <v>1</v>
-      </c>
-      <c r="B5" s="1">
-        <v>2</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="1">
-        <v>550</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1">
-        <v>49000</v>
-      </c>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
-        <v>9</v>
-      </c>
-      <c r="B6" s="1">
-        <v>2</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="1">
-        <v>2000</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1">
-        <v>24000</v>
-      </c>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
-        <v>1</v>
-      </c>
-      <c r="B7" s="1">
-        <v>3</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="1">
-        <v>1200</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1">
-        <v>39000</v>
-      </c>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
-        <v>9</v>
-      </c>
-      <c r="B8" s="1">
-        <v>3</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="1">
-        <v>1200</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1">
-        <v>39000</v>
-      </c>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
-        <v>1</v>
-      </c>
-      <c r="B9" s="1">
-        <v>4</v>
-      </c>
-      <c r="C9" s="1" t="s">
+      <c r="G11" s="3"/>
+      <c r="H11" s="3">
+        <v>19000</v>
+      </c>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="1">
-        <v>550</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1">
-        <v>39000</v>
-      </c>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10" s="1">
-        <v>9</v>
-      </c>
-      <c r="B10" s="1">
-        <v>4</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="1">
-        <v>550</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1">
-        <v>39000</v>
-      </c>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="M10" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11" s="1">
-        <v>10</v>
-      </c>
-      <c r="B11" s="1">
-        <v>1</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" s="1">
-        <v>5800</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1">
-        <v>19000</v>
-      </c>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1" t="s">
+      <c r="N11" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="M11" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>1</v>
       </c>
       <c r="B12" s="1">
         <v>5</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D12" s="1">
+      <c r="C12" s="1">
+        <v>7</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="1">
         <v>120</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1">
+      <c r="F12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1">
         <v>39900</v>
       </c>
-      <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
-      <c r="L12" s="1" t="s">
+      <c r="L12" s="1"/>
+      <c r="M12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N12" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="M12" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>1</v>
       </c>
       <c r="B13" s="2">
         <v>6</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="1"/>
+      <c r="D13" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" s="2">
+        <v>2400</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="2">
-        <v>2400</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2">
+      <c r="G13" s="2"/>
+      <c r="H13" s="2">
         <v>27000</v>
       </c>
-      <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
-      <c r="L13" s="2" t="s">
+      <c r="L13" s="2"/>
+      <c r="M13" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="N13" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="M13" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
+      <c r="C14" s="1"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
@@ -998,12 +1069,15 @@
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
-      <c r="L14" s="2" t="s">
+      <c r="L14" s="2"/>
+      <c r="M14" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="N14" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="M14" s="2" t="s">
-        <v>40</v>
-      </c>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>